<commit_message>
Merge after pull requests
</commit_message>
<xml_diff>
--- a/ScreenResolution.xlsx
+++ b/ScreenResolution.xlsx
@@ -21,6 +21,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Sunmi V1s</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,84 +344,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G6"/>
+  <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>424</v>
+        <v>240</v>
       </c>
       <c r="C2">
         <f>B2*B2</f>
-        <v>179776</v>
+        <v>57600</v>
       </c>
       <c r="F2">
         <f>G2*G2</f>
-        <v>179776</v>
+        <v>129600</v>
       </c>
       <c r="G2">
-        <v>424</v>
+        <v>360</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>848</v>
+        <v>427</v>
       </c>
       <c r="C3">
         <f>B3*B3</f>
-        <v>719104</v>
+        <v>182329</v>
       </c>
       <c r="F3">
         <f>G3*G3</f>
-        <v>719104</v>
+        <v>409600</v>
       </c>
       <c r="G3">
-        <v>848</v>
+        <v>640</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D4">
         <f>C2+C3</f>
-        <v>898880</v>
+        <v>239929</v>
       </c>
       <c r="E4">
         <f>F2+F3</f>
-        <v>898880</v>
+        <v>539200</v>
+      </c>
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>360</v>
+      </c>
+      <c r="K4">
+        <v>640</v>
+      </c>
+      <c r="L4">
+        <v>4.1225529999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D5">
         <f>SQRT(D4)</f>
-        <v>948.09282245991085</v>
+        <v>489.82547912496346</v>
       </c>
       <c r="E5">
         <f>SQRT(E4)</f>
-        <v>948.09282245991085</v>
+        <v>734.30239002743281</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6">
-        <v>5.99</v>
+        <v>2.75</v>
       </c>
       <c r="D6">
         <f>D5/C6</f>
-        <v>158.27926919197176</v>
+        <v>178.11835604544126</v>
       </c>
       <c r="E6">
         <f>D6</f>
-        <v>158.27926919197176</v>
+        <v>178.11835604544126</v>
       </c>
       <c r="F6">
         <f>E5/E6</f>
-        <v>5.99</v>
+        <v>4.1225531513444844</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>